<commit_message>
Updated the requested changes from Keyur as below. - Need to update weight with double DataType - Need to bring log up as failure message can display first - User credential must come from  same excel, but different sheet - Removed unnecessary waits
</commit_message>
<xml_diff>
--- a/Resources/CFL_Data.xlsx
+++ b/Resources/CFL_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\CFL\workspace\CFAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520A761E-4D43-4B45-A792-B53E73E89FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72646AD-2F99-4EC9-8ED7-DE611E2D8ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FAB0F961-D505-42B6-B675-3AE2B5618F1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FAB0F961-D505-42B6-B675-3AE2B5618F1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Batch" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Credentials" sheetId="3" r:id="rId1"/>
+    <sheet name="Create Batch" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -243,6 +244,27 @@
   <si>
     <t>THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENTTHIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENTTHIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENTTHIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENTTHIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT THIS TEST COMMENT</t>
   </si>
+  <si>
+    <t>Source Site Username</t>
+  </si>
+  <si>
+    <t>Source Site Password</t>
+  </si>
+  <si>
+    <t>Receiving Site Username</t>
+  </si>
+  <si>
+    <t>Receiving Site Password</t>
+  </si>
+  <si>
+    <t>C1e@nFi1l</t>
+  </si>
+  <si>
+    <t>Fill_Site_User1@grr.la</t>
+  </si>
+  <si>
+    <t>Source_Site_User1@grr.la</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +313,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -346,6 +380,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -661,12 +700,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A6E41-2504-4635-9009-03BDA1460376}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{FA50C767-9D13-4112-8EE6-4298733758EB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA647E-5043-40A7-85A8-20186CBF4D95}">
   <dimension ref="A1:XFD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17192,7 +17291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BC81F0-AA07-42D6-BF99-68B22C41F83D}">
   <dimension ref="A1:G12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed Edit Batch Information test cases
</commit_message>
<xml_diff>
--- a/Resources/CFL_Data.xlsx
+++ b/Resources/CFL_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\CFL\workspace\CFAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72646AD-2F99-4EC9-8ED7-DE611E2D8ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E4BCD5-AD00-4391-B5AF-DCF1698B4BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FAB0F961-D505-42B6-B675-3AE2B5618F1D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>#</t>
   </si>
@@ -264,6 +264,35 @@
   </si>
   <si>
     <t>Source_Site_User1@grr.la</t>
+  </si>
+  <si>
+    <t>OTHER_SOURCE_TYPE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SOURCE_TYPE
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Only enter if selected Others)</t>
+    </r>
+  </si>
+  <si>
+    <t>Ex Situ Excavation</t>
+  </si>
+  <si>
+    <t>In Situ Excavation</t>
+  </si>
+  <si>
+    <t>Test Source Type Other</t>
   </si>
 </sst>
 </file>
@@ -765,7 +794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA647E-5043-40A7-85A8-20186CBF4D95}">
   <dimension ref="A1:XFD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -776,14 +807,16 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="13" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="33.28515625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="81.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="15" width="21.85546875" customWidth="1"/>
+    <col min="16" max="16" width="32.140625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="33.28515625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="81.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -809,34 +842,38 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1"/>
-      <c r="R1"/>
       <c r="S1"/>
       <c r="T1"/>
       <c r="U1"/>
@@ -17209,7 +17246,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>44114</v>
+        <v>44119</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>44</v>
@@ -17227,40 +17264,46 @@
         <v>1000000</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" location="gfe_rd=cr&amp;gws_rd=ssl" xr:uid="{57A0EF76-6D46-46A8-B4BB-467C41FA0404}"/>
+    <hyperlink ref="Q2" r:id="rId1" location="gfe_rd=cr&amp;gws_rd=ssl" xr:uid="{57A0EF76-6D46-46A8-B4BB-467C41FA0404}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3044EA52-DF59-45D5-A4A5-A5882627091B}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
@@ -17271,19 +17314,25 @@
           <x14:formula1>
             <xm:f>Sheet2!$C$1:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{54AF2CE2-1818-4C9E-8185-09B2047376B6}">
           <x14:formula1>
             <xm:f>Sheet2!$E$1:$E$12</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B02A8259-FAF8-416D-9B8F-5F358E205546}">
           <x14:formula1>
             <xm:f>Sheet2!$G$1:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>N2:N1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86806161-9707-4994-98BC-8B600BC2FC01}">
+          <x14:formula1>
+            <xm:f>Sheet2!$I$1:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -17293,10 +17342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BC81F0-AA07-42D6-BF99-68B22C41F83D}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17307,9 +17356,11 @@
     <col min="5" max="5" width="30.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="3.140625" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -17322,8 +17373,11 @@
       <c r="G1" t="s">
         <v>36</v>
       </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -17336,8 +17390,11 @@
       <c r="G2" t="s">
         <v>37</v>
       </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>30</v>
       </c>
@@ -17347,8 +17404,11 @@
       <c r="G3" t="s">
         <v>38</v>
       </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>31</v>
       </c>
@@ -17359,7 +17419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>32</v>
       </c>
@@ -17370,7 +17430,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>33</v>
       </c>
@@ -17381,7 +17441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
@@ -17389,7 +17449,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
         <v>23</v>
       </c>
@@ -17397,22 +17457,22 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
- Completed Source Site Registration Test Cases
</commit_message>
<xml_diff>
--- a/Resources/CFL_Data.xlsx
+++ b/Resources/CFL_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\CFL\workspace\CFAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E4BCD5-AD00-4391-B5AF-DCF1698B4BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36EFA70-EF36-429A-A869-78BC30004ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FAB0F961-D505-42B6-B675-3AE2B5618F1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="3" r:id="rId1"/>
     <sheet name="Create Batch" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -230,9 +230,6 @@
     </r>
   </si>
   <si>
-    <t>TESTTEST001</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -286,13 +283,19 @@
     </r>
   </si>
   <si>
-    <t>Ex Situ Excavation</t>
+    <t>Test Source Type Other</t>
   </si>
   <si>
-    <t>In Situ Excavation</t>
+    <t>Stockpile</t>
   </si>
   <si>
-    <t>Test Source Type Other</t>
+    <t>Excavation</t>
+  </si>
+  <si>
+    <t>Drill Spoils</t>
+  </si>
+  <si>
+    <t>TESTTEST10252020</t>
   </si>
 </sst>
 </file>
@@ -744,18 +747,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,18 +767,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -794,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DA647E-5043-40A7-85A8-20186CBF4D95}">
   <dimension ref="A1:XFD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,10 +845,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>7</v>
@@ -17246,10 +17249,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>44119</v>
+        <v>44129</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>3</v>
@@ -17264,10 +17267,10 @@
         <v>1000000</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>28</v>
@@ -17283,16 +17286,16 @@
         <v>33</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="R2" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -17330,7 +17333,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86806161-9707-4994-98BC-8B600BC2FC01}">
           <x14:formula1>
-            <xm:f>Sheet2!$I$1:$I$3</xm:f>
+            <xm:f>Sheet2!$I$1:$I$4</xm:f>
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
@@ -17345,7 +17348,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17405,7 +17408,7 @@
         <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -17417,6 +17420,9 @@
       </c>
       <c r="G4" t="s">
         <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Latest Test execution completed with the updated test cases.
</commit_message>
<xml_diff>
--- a/Resources/CFL_Data.xlsx
+++ b/Resources/CFL_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Work\GFL\CFL\workspace\CFAutomation\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36EFA70-EF36-429A-A869-78BC30004ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CAEFC3-DF38-489C-A4C1-4469AF1EF986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FAB0F961-D505-42B6-B675-3AE2B5618F1D}"/>
   </bookViews>
@@ -295,7 +295,7 @@
     <t>Drill Spoils</t>
   </si>
   <si>
-    <t>TESTTEST10252020</t>
+    <t>TESTTEST110520204</t>
   </si>
 </sst>
 </file>
@@ -17249,7 +17249,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <v>44129</v>
+        <v>44140</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>61</v>
@@ -17258,13 +17258,13 @@
         <v>3</v>
       </c>
       <c r="E2" s="5">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="F2" s="5">
-        <v>20000</v>
+        <v>20</v>
       </c>
       <c r="G2" s="5">
-        <v>1000000</v>
+        <v>100</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>58</v>

</xml_diff>